<commit_message>
Veri tabanı yedeği güncellendi
</commit_message>
<xml_diff>
--- a/tools/import/CIVATALAR.xlsx
+++ b/tools/import/CIVATALAR.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="317">
   <si>
     <t>150.05.0501.00001</t>
   </si>
@@ -964,6 +964,12 @@
   </si>
   <si>
     <t xml:space="preserve">Alış Fiyatı-1   </t>
+  </si>
+  <si>
+    <t>150.05.0511.00001</t>
+  </si>
+  <si>
+    <t>M5X10 YILDIZ HAVSABAS CIVATA</t>
   </si>
 </sst>
 </file>
@@ -1338,11 +1344,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
@@ -6629,6 +6649,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>315</v>
+      </c>
+      <c r="B152" t="s">
+        <v>316</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>